<commit_message>
Working on Comp 230 TDD
</commit_message>
<xml_diff>
--- a/Python/Comp 230/datasheet.xlsx
+++ b/Python/Comp 230/datasheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\cohort4\Python\Comp 230\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA99B4E9-2A5D-4781-826D-A048B10FE57C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A01FE63-4D08-40B9-AE6C-BE166DFFC04E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="821" xr2:uid="{372980B3-46BC-4154-BAD1-391F1841EC37}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="821" activeTab="1" xr2:uid="{372980B3-46BC-4154-BAD1-391F1841EC37}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Invoice Line Items" sheetId="4" r:id="rId3"/>
     <sheet name="Product" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -872,7 +872,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -898,7 +898,6 @@
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1227,7 +1226,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F05B71BE-0CED-4523-891D-2E543392AF3E}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
@@ -2064,10 +2063,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8FC37B8-3CDA-4090-955F-0F1D8074295B}">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2076,7 +2075,7 @@
     <col min="5" max="5" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2" t="s">
@@ -2084,7 +2083,7 @@
       </c>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -2100,14 +2099,12 @@
       <c r="E2" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -2120,18 +2117,15 @@
       <c r="D3" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="E3" s="14">
-        <f>SUM(260+210)</f>
+      <c r="E3" s="13">
         <v>470</v>
       </c>
+      <c r="F3" s="3"/>
       <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="H3" s="12"/>
       <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="3"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -2144,18 +2138,15 @@
       <c r="D4" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="13">
         <v>1282.5</v>
       </c>
-      <c r="F4" s="9"/>
+      <c r="F4" s="3"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+      <c r="H4" s="12"/>
       <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="3"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -2168,18 +2159,15 @@
       <c r="D5" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="13">
         <v>210</v>
       </c>
-      <c r="F5" s="9"/>
+      <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+      <c r="H5" s="8"/>
       <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="3"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -2192,18 +2180,15 @@
       <c r="D6" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="13">
         <v>464.5</v>
       </c>
-      <c r="F6" s="9"/>
+      <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="H6" s="8"/>
       <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="3"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -2216,18 +2201,15 @@
       <c r="D7" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="13">
         <v>136</v>
       </c>
-      <c r="F7" s="9"/>
+      <c r="F7" s="3"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="H7" s="8"/>
       <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="3"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -2240,18 +2222,15 @@
       <c r="D8" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="13">
         <v>1303.5</v>
       </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="8"/>
       <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="3"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -2264,18 +2243,15 @@
       <c r="D9" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="13">
         <v>150.5</v>
       </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="11"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="10"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -2288,18 +2264,15 @@
       <c r="D10" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="13">
         <v>200</v>
       </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="11"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="10"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -2312,222 +2285,187 @@
       <c r="D11" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="13">
         <v>675</v>
       </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="11"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="10"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="11"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="10"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="11"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="10"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="11"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="10"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="11"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="10"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="11"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="10"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="11"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="10"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="11"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="10"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="11"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="10"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="11"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="10"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="11"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="10"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="11"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="10"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="11"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="10"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="11"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="10"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="11"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="10"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="11"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="10"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
+      <c r="F27" s="3"/>
       <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="11"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H27" s="8"/>
+      <c r="I27" s="10"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
     </row>
   </sheetData>
@@ -2540,15 +2478,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2A2651B-E973-4A98-A7C3-94E414BA7596}">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2557,10 +2495,8 @@
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>19</v>
       </c>
@@ -2579,9 +2515,8 @@
       <c r="F2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -2594,20 +2529,18 @@
       <c r="D3" s="3">
         <v>13</v>
       </c>
-      <c r="E3" s="13">
-        <f>13*20</f>
+      <c r="E3" s="12">
         <v>260</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="8"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="8"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -2620,20 +2553,18 @@
       <c r="D4" s="3">
         <v>14</v>
       </c>
-      <c r="E4" s="13">
-        <f>14*15</f>
+      <c r="E4" s="12">
         <v>210</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="8"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="8"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -2647,19 +2578,17 @@
         <v>15</v>
       </c>
       <c r="E5" s="8">
-        <f>15*45</f>
         <v>675</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="8"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="8"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -2673,19 +2602,17 @@
         <v>11</v>
       </c>
       <c r="E6" s="8">
-        <f>11*35</f>
         <v>385</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="8"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="8"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -2699,19 +2626,17 @@
         <v>8</v>
       </c>
       <c r="E7" s="8">
-        <f>8*25</f>
         <v>200</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="8"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="8"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -2725,19 +2650,17 @@
         <v>9</v>
       </c>
       <c r="E8" s="8">
-        <f>9*2.5</f>
         <v>22.5</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="8"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="8"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -2751,19 +2674,17 @@
         <v>9</v>
       </c>
       <c r="E9" s="8">
-        <f>9*10</f>
         <v>90</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="10">
         <v>43898</v>
       </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="8"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="8"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -2777,19 +2698,17 @@
         <v>8</v>
       </c>
       <c r="E10" s="8">
-        <f>8*15</f>
         <v>120</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="10">
         <v>43898</v>
       </c>
-      <c r="H10" s="6"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="8"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -2803,19 +2722,17 @@
         <v>13</v>
       </c>
       <c r="E11" s="8">
-        <f>13*8</f>
         <v>104</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="10">
         <v>43914</v>
       </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="8"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -2829,19 +2746,17 @@
         <v>9</v>
       </c>
       <c r="E12" s="8">
-        <f>9*35</f>
         <v>315</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="10">
         <v>43914</v>
       </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="8"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="8"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -2855,19 +2770,17 @@
         <v>13</v>
       </c>
       <c r="E13" s="8">
-        <f>13*3.5</f>
         <v>45.5</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="10">
         <v>43914</v>
       </c>
-      <c r="H13" s="6"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="8"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="8"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -2881,19 +2794,17 @@
         <v>11</v>
       </c>
       <c r="E14" s="8">
-        <f>11*10</f>
         <v>110</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="10">
         <v>43915</v>
       </c>
-      <c r="H14" s="6"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="8"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="8"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -2907,19 +2818,17 @@
         <v>4</v>
       </c>
       <c r="E15" s="8">
-        <f>4*6.5</f>
         <v>26</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="10">
         <v>43915</v>
       </c>
-      <c r="H15" s="6"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="8"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="8"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -2933,19 +2842,17 @@
         <v>2</v>
       </c>
       <c r="E16" s="8">
-        <f>2*5.5</f>
         <v>11</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="10">
         <v>43923</v>
       </c>
-      <c r="H16" s="6"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="8"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="8"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -2959,19 +2866,17 @@
         <v>5</v>
       </c>
       <c r="E17" s="8">
-        <f>5*8.5</f>
         <v>42.5</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="10">
         <v>43923</v>
       </c>
-      <c r="H17" s="6"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="8"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="8"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -2985,14 +2890,13 @@
         <v>10</v>
       </c>
       <c r="E18" s="8">
-        <f>10*45</f>
         <v>450</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="10">
         <v>43923</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -3006,14 +2910,13 @@
         <v>20</v>
       </c>
       <c r="E19" s="8">
-        <f>20*35</f>
         <v>700</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="10">
         <v>43923</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -3027,14 +2930,13 @@
         <v>4</v>
       </c>
       <c r="E20" s="8">
-        <f>4*25</f>
         <v>100</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F20" s="10">
         <v>43923</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -3048,14 +2950,13 @@
         <v>13</v>
       </c>
       <c r="E21" s="8">
-        <f>13*6.5</f>
         <v>84.5</v>
       </c>
-      <c r="F21" s="11">
+      <c r="F21" s="10">
         <v>43929</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -3069,14 +2970,13 @@
         <v>12</v>
       </c>
       <c r="E22" s="8">
-        <f>12*5.5</f>
         <v>66</v>
       </c>
-      <c r="F22" s="11">
+      <c r="F22" s="10">
         <v>43929</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -3090,14 +2990,13 @@
         <v>10</v>
       </c>
       <c r="E23" s="8">
-        <f>10*5.5</f>
         <v>55</v>
       </c>
-      <c r="F23" s="11">
+      <c r="F23" s="10">
         <v>43933</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>22</v>
       </c>
@@ -3111,14 +3010,13 @@
         <v>10</v>
       </c>
       <c r="E24" s="8">
-        <f>10*2.5</f>
         <v>25</v>
       </c>
-      <c r="F24" s="11">
+      <c r="F24" s="10">
         <v>43933</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -3132,14 +3030,13 @@
         <v>8</v>
       </c>
       <c r="E25" s="8">
-        <f>8*15</f>
         <v>120</v>
       </c>
-      <c r="F25" s="11">
+      <c r="F25" s="10">
         <v>43933</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>24</v>
       </c>
@@ -3153,14 +3050,13 @@
         <v>13</v>
       </c>
       <c r="E26" s="8">
-        <f>13*45</f>
         <v>585</v>
       </c>
-      <c r="F26" s="11">
+      <c r="F26" s="10">
         <v>43936</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>25</v>
       </c>
@@ -3174,27 +3070,26 @@
         <v>9</v>
       </c>
       <c r="E27" s="8">
-        <f>9*10</f>
         <v>90</v>
       </c>
-      <c r="F27" s="11">
+      <c r="F27" s="10">
         <v>43936</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="D28" s="10"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="D29" s="10"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="D30" s="10"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="D31" s="10"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="D32" s="10"/>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D28" s="9"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D29" s="9"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D30" s="9"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D31" s="9"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D32" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>